<commit_message>
10 20 percent iris
</commit_message>
<xml_diff>
--- a/Iris_Rank_filtering_implementation.xlsx
+++ b/Iris_Rank_filtering_implementation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shukl\Documents\GitHub\Decision-Trees\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3213431E-906D-4324-82D8-9F21D0BC1930}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FC6F5E7-A7AB-40E2-AC26-A47BE2BB0893}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="823" firstSheet="9" activeTab="17" xr2:uid="{6C67A883-E7E1-4B49-B51F-4602C047CF2B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="823" firstSheet="9" activeTab="16" xr2:uid="{6C67A883-E7E1-4B49-B51F-4602C047CF2B}"/>
   </bookViews>
   <sheets>
     <sheet name="IRIS_DT_DIST80" sheetId="8" state="hidden" r:id="rId1"/>
@@ -7980,8 +7980,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DE34F46-5B5F-40B1-84FA-2526652B640D}">
   <dimension ref="A1:N11"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A2" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -8152,19 +8152,19 @@
         <v>0</v>
       </c>
       <c r="J6" s="144">
-        <v>0.96132600000000001</v>
+        <v>0.93922700000000003</v>
       </c>
       <c r="K6" s="145">
-        <v>3.8674E-2</v>
+        <v>6.0773000000000001E-2</v>
       </c>
       <c r="L6" s="143">
-        <v>1.6574999999999999E-2</v>
+        <v>0</v>
       </c>
       <c r="M6" s="144">
-        <v>0.94475100000000001</v>
+        <v>0.93370200000000003</v>
       </c>
       <c r="N6" s="145">
-        <v>3.8674E-2</v>
+        <v>6.6297999999999996E-2</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="15" thickBot="1">
@@ -8203,10 +8203,10 @@
         <v>0</v>
       </c>
       <c r="M7" s="147">
-        <v>4.8386999999999999E-2</v>
+        <v>4.3011000000000001E-2</v>
       </c>
       <c r="N7" s="148">
-        <v>0.95161300000000004</v>
+        <v>0.95698899999999998</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="15" thickBot="1">
@@ -8252,7 +8252,7 @@
         <v>1</v>
       </c>
       <c r="J9" s="153">
-        <v>0.96099999999999997</v>
+        <v>0.93899999999999995</v>
       </c>
       <c r="K9" s="154">
         <v>0.98399999999999999</v>
@@ -8261,10 +8261,10 @@
         <v>1</v>
       </c>
       <c r="M9" s="153">
-        <v>0.94499999999999995</v>
+        <v>0.93400000000000005</v>
       </c>
       <c r="N9" s="154">
-        <v>0.95199999999999996</v>
+        <v>0.95699999999999996</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="15" thickBot="1">
@@ -8299,16 +8299,16 @@
         <v>8.9999999999999993E-3</v>
       </c>
       <c r="K10" s="157">
-        <v>0.02</v>
+        <v>3.2000000000000001E-2</v>
       </c>
       <c r="L10" s="155">
-        <v>8.0000000000000002E-3</v>
+        <v>0</v>
       </c>
       <c r="M10" s="156">
-        <v>2.5999999999999999E-2</v>
+        <v>2.3E-2</v>
       </c>
       <c r="N10" s="157">
-        <v>0.02</v>
+        <v>3.5000000000000003E-2</v>
       </c>
     </row>
     <row r="11" spans="1:14">
@@ -8343,8 +8343,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8628703-0CAA-4F07-98E5-96A9CD16B317}">
   <dimension ref="A1:M10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L20" sqref="L20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -8508,19 +8508,19 @@
         <v>0</v>
       </c>
       <c r="I6" s="144">
-        <v>0.93922700000000003</v>
+        <v>0.96132600000000001</v>
       </c>
       <c r="J6" s="145">
-        <v>6.0773000000000001E-2</v>
+        <v>3.8674E-2</v>
       </c>
       <c r="K6" s="143">
-        <v>0</v>
+        <v>1.6574999999999999E-2</v>
       </c>
       <c r="L6" s="144">
-        <v>0.93370200000000003</v>
+        <v>0.94475100000000001</v>
       </c>
       <c r="M6" s="145">
-        <v>6.6297999999999996E-2</v>
+        <v>3.8674E-2</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="15" thickBot="1">
@@ -8558,10 +8558,10 @@
         <v>0</v>
       </c>
       <c r="L7" s="147">
-        <v>4.3011000000000001E-2</v>
+        <v>4.8386999999999999E-2</v>
       </c>
       <c r="M7" s="148">
-        <v>0.95698899999999998</v>
+        <v>0.95161300000000004</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="15" thickBot="1">
@@ -8604,7 +8604,7 @@
         <v>1</v>
       </c>
       <c r="I9" s="153">
-        <v>0.93899999999999995</v>
+        <v>0.96099999999999997</v>
       </c>
       <c r="J9" s="154">
         <v>0.98399999999999999</v>
@@ -8613,10 +8613,10 @@
         <v>1</v>
       </c>
       <c r="L9" s="153">
-        <v>0.93400000000000005</v>
+        <v>0.94499999999999995</v>
       </c>
       <c r="M9" s="154">
-        <v>0.95699999999999996</v>
+        <v>0.95199999999999996</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="15" thickBot="1">
@@ -8648,16 +8648,16 @@
         <v>8.9999999999999993E-3</v>
       </c>
       <c r="J10" s="157">
-        <v>3.2000000000000001E-2</v>
+        <v>0.02</v>
       </c>
       <c r="K10" s="155">
-        <v>0</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="L10" s="156">
-        <v>2.3E-2</v>
+        <v>2.5999999999999999E-2</v>
       </c>
       <c r="M10" s="157">
-        <v>3.5000000000000003E-2</v>
+        <v>0.02</v>
       </c>
     </row>
   </sheetData>

</xml_diff>